<commit_message>
adding the root endpoint
</commit_message>
<xml_diff>
--- a/database/order_data.xlsx
+++ b/database/order_data.xlsx
@@ -7525,6 +7525,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -7730,8 +7734,8 @@
   </sheetPr>
   <dimension ref="A1:I2476"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1077" workbookViewId="0">
-      <selection activeCell="B1101" sqref="B1101"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
adding three more intents
</commit_message>
<xml_diff>
--- a/database/order_data.xlsx
+++ b/database/order_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://utoronto-my.sharepoint.com/personal/ericjs_yu_mail_utoronto_ca/Documents/Desktop/AI_Kata_backend/database/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="11_A0103AC7DCC273F304B651D5D02528E350D23F5B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{48149E10-919D-4AFE-9B37-050FD594EF8B}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="11_A0103AC7DCC273F304B651D5D02528E350D23F5B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3C2AF390-0180-4FD0-B680-E175840E5AEE}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -7734,13 +7734,14 @@
   </sheetPr>
   <dimension ref="A1:I2476"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="40.44140625" customWidth="1"/>
+    <col min="9" max="9" width="19.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>